<commit_message>
Aanpassing referentieregios en enkele andere zaken
Closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/43 : indien naam wijk = naam gemeente, maak er van "Naam (wijk)"
Closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/44 : Naamwijziging statsec
Closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/45 : vraag om Brussel+Vlaanderen toe te voegen
Closes https://github.com/provinciesincijfers/gebiedsniveaus/issues/46 : aanpassing referentieregio's
</commit_message>
<xml_diff>
--- a/data_voor_swing/aggregatietabellen/refreg_provincie.xlsx
+++ b/data_voor_swing/aggregatietabellen/refreg_provincie.xlsx
@@ -382,7 +382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,36 +537,46 @@
         </is>
       </c>
       <c r="B15" s="23">
-        <v>40000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="0" outlineLevel="0">
       <c r="A16" t="inlineStr">
         <is>
-          <t>REFREG15</t>
+          <t>REFREG14</t>
         </is>
       </c>
       <c r="B16" s="23">
-        <v>70000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="0" outlineLevel="0">
       <c r="A17" t="inlineStr">
         <is>
-          <t>REFREG91</t>
+          <t>REFREG15</t>
         </is>
       </c>
       <c r="B17" s="23">
-        <v>99991</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="0" outlineLevel="0">
       <c r="A18" t="inlineStr">
         <is>
+          <t>REFREG91</t>
+        </is>
+      </c>
+      <c r="B18" s="23">
+        <v>99991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="0" outlineLevel="0">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>REFREG99</t>
         </is>
       </c>
-      <c r="B18" s="23">
+      <c r="B19" s="23">
         <v>99999</v>
       </c>
     </row>

</xml_diff>